<commit_message>
Correct One Header in Spreadsheet
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Float</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Inline, using types.h</t>
-  </si>
-  <si>
-    <t>Uno/Pro</t>
   </si>
   <si>
     <t>vs Int</t>
@@ -440,11 +437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45779968"/>
-        <c:axId val="45781760"/>
+        <c:axId val="104930304"/>
+        <c:axId val="104936192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45779968"/>
+        <c:axId val="104930304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -456,12 +453,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45781760"/>
+        <c:crossAx val="104936192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45781760"/>
+        <c:axId val="104936192"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -474,7 +471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45779968"/>
+        <c:crossAx val="104930304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45805952"/>
-        <c:axId val="45807488"/>
+        <c:axId val="104961920"/>
+        <c:axId val="104963456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45805952"/>
+        <c:axId val="104961920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -832,12 +829,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45807488"/>
+        <c:crossAx val="104963456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45807488"/>
+        <c:axId val="104963456"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -849,7 +846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45805952"/>
+        <c:crossAx val="104961920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1405,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1429,7 +1426,7 @@
         <v>Arduino M0 Pro</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>23</v>
@@ -1475,13 +1472,13 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -1502,7 +1499,7 @@
         <v>9.26</v>
       </c>
       <c r="G5">
-        <f>C5/D5</f>
+        <f t="shared" ref="G5:G10" si="0">C5/D5</f>
         <v>2.632450331125828</v>
       </c>
       <c r="H5">
@@ -1510,7 +1507,7 @@
         <v>8.5853131749460037</v>
       </c>
       <c r="K5">
-        <f>D5/E5</f>
+        <f t="shared" ref="K5:K12" si="1">D5/E5</f>
         <v>3.2613390928725701</v>
       </c>
     </row>
@@ -1532,15 +1529,15 @@
         <v>19</v>
       </c>
       <c r="G6">
-        <f>C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.6076884337753903</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H10" si="0">C6/E6</f>
+        <f t="shared" ref="H6:H10" si="2">C6/E6</f>
         <v>8.1757894736842101</v>
       </c>
       <c r="K6">
-        <f>D6/E6</f>
+        <f t="shared" si="1"/>
         <v>3.135263157894737</v>
       </c>
     </row>
@@ -1562,15 +1559,15 @@
         <v>38.44</v>
       </c>
       <c r="G7">
-        <f>C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2.6091293322062556</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.0296566077003124</v>
       </c>
       <c r="K7">
-        <f>D7/E7</f>
+        <f t="shared" si="1"/>
         <v>3.0775234131113423</v>
       </c>
     </row>
@@ -1592,15 +1589,15 @@
         <v>77.28</v>
       </c>
       <c r="G8">
-        <f>C8/D8</f>
+        <f t="shared" si="0"/>
         <v>2.6716595744680851</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1242236024844718</v>
       </c>
       <c r="K8">
-        <f>D8/E8</f>
+        <f t="shared" si="1"/>
         <v>3.0408902691511388</v>
       </c>
     </row>
@@ -1622,15 +1619,15 @@
         <v>154.91999999999999</v>
       </c>
       <c r="G9">
-        <f>C9/D9</f>
+        <f t="shared" si="0"/>
         <v>2.7124735729386891</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.2816937774335155</v>
       </c>
       <c r="K9">
-        <f>D9/E9</f>
+        <f t="shared" si="1"/>
         <v>3.0531887425768143</v>
       </c>
     </row>
@@ -1652,15 +1649,15 @@
         <v>310.14999999999998</v>
       </c>
       <c r="G10">
-        <f>C10/D10</f>
+        <f t="shared" si="0"/>
         <v>2.7798941798941801</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.4700951152668065</v>
       </c>
       <c r="K10">
-        <f>D10/E10</f>
+        <f t="shared" si="1"/>
         <v>3.0469127841367083</v>
       </c>
     </row>
@@ -1682,7 +1679,7 @@
         <v>620.58000000000004</v>
       </c>
       <c r="K11">
-        <f>D11/E11</f>
+        <f t="shared" si="1"/>
         <v>3.0407038576815237</v>
       </c>
     </row>
@@ -1704,7 +1701,7 @@
         <v>1241.3699999999999</v>
       </c>
       <c r="K12">
-        <f>D12/E12</f>
+        <f t="shared" si="1"/>
         <v>3.0297171673231995</v>
       </c>
     </row>
@@ -1752,7 +1749,7 @@
         <v>8000</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" ref="D18:D21" si="1">1/C18*1000000</f>
+        <f t="shared" ref="D18:D21" si="3">1/C18*1000000</f>
         <v>125</v>
       </c>
     </row>
@@ -1761,7 +1758,7 @@
         <v>11025</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90.702947845804985</v>
       </c>
     </row>
@@ -1770,7 +1767,7 @@
         <v>22050</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45.351473922902493</v>
       </c>
       <c r="E20" s="4"/>
@@ -1786,7 +1783,7 @@
         <v>44100</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22.675736961451246</v>
       </c>
       <c r="E21" s="4"/>
@@ -1807,7 +1804,7 @@
         <v>Arduino M0 Pro</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23">
         <f>48/16</f>
@@ -1858,22 +1855,22 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
         <v>29</v>
       </c>
-      <c r="H25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" t="s">
-        <v>30</v>
-      </c>
       <c r="L25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1898,7 +1895,7 @@
         <v>38.44</v>
       </c>
       <c r="G26">
-        <f>C26/D26</f>
+        <f t="shared" ref="G26:G37" si="4">C26/D26</f>
         <v>2.3994661921708182</v>
       </c>
       <c r="H26">
@@ -1940,19 +1937,19 @@
         <v>77.28</v>
       </c>
       <c r="G27">
-        <f>C27/D27</f>
+        <f t="shared" si="4"/>
         <v>2.4459886854648314</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H37" si="2">C27/E27</f>
+        <f t="shared" ref="H27:H37" si="5">C27/E27</f>
         <v>7.1053312629399592</v>
       </c>
       <c r="I27">
-        <f t="shared" ref="I27:I37" si="3">D27/E27</f>
+        <f t="shared" ref="I27:I37" si="6">D27/E27</f>
         <v>2.9048913043478262</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27:K29" si="4">C27/C35</f>
+        <f t="shared" ref="K27:K29" si="7">C27/C35</f>
         <v>6.9842279318239635</v>
       </c>
       <c r="L27">
@@ -1960,7 +1957,7 @@
         <v>8.6542020046260593</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M29" si="5">E27/E35</f>
+        <f t="shared" ref="M27:M29" si="8">E27/E35</f>
         <v>6.6563307493540051</v>
       </c>
     </row>
@@ -1982,19 +1979,19 @@
         <v>154.91999999999999</v>
       </c>
       <c r="G28">
-        <f>C28/D28</f>
+        <f t="shared" si="4"/>
         <v>2.4946388698516571</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.2837593596695083</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.9197650400206561</v>
       </c>
       <c r="K28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.2659368963296842</v>
       </c>
       <c r="L28">
@@ -2002,7 +1999,7 @@
         <v>8.3826908821349146</v>
       </c>
       <c r="M28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.8066783831282942</v>
       </c>
     </row>
@@ -2024,19 +2021,19 @@
         <v>310.14999999999998</v>
       </c>
       <c r="G29">
-        <f>C29/D29</f>
+        <f t="shared" si="4"/>
         <v>2.5816660764872523</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.5221666935353868</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.9136869256811222</v>
       </c>
       <c r="K29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.5746753246753249</v>
       </c>
       <c r="L29">
@@ -2044,7 +2041,7 @@
         <v>8.4188559716787772</v>
       </c>
       <c r="M29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.8830448291167325</v>
       </c>
     </row>
@@ -2070,15 +2067,15 @@
         <v>6.04</v>
       </c>
       <c r="G30">
-        <f>C30/D30</f>
+        <f t="shared" si="4"/>
         <v>9.0346907993966816</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>19.834437086092716</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.1953642384105958</v>
       </c>
       <c r="K30">
@@ -2096,7 +2093,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="B31">
-        <f t="shared" ref="B31:B37" si="6">B27</f>
+        <f t="shared" ref="B31:B37" si="9">B27</f>
         <v>32</v>
       </c>
       <c r="C31" s="4">
@@ -2112,19 +2109,19 @@
         <v>11.61</v>
       </c>
       <c r="G31">
-        <f>C31/D31</f>
+        <f t="shared" si="4"/>
         <v>9.1187355435620656</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20.373815676141259</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.2342807924203276</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:K33" si="7">C31/C35</f>
+        <f t="shared" ref="K31:K33" si="10">C31/C35</f>
         <v>3.0086491986771811</v>
       </c>
       <c r="L31">
@@ -2132,13 +2129,13 @@
         <v>1</v>
       </c>
       <c r="M31">
-        <f t="shared" ref="M31:M33" si="8">E31/E35</f>
+        <f t="shared" ref="M31:M33" si="11">E31/E35</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="B32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="C32" s="4">
@@ -2154,19 +2151,19 @@
         <v>22.76</v>
       </c>
       <c r="G32">
-        <f>C32/D32</f>
+        <f t="shared" si="4"/>
         <v>8.7085417824717446</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20.650263620386642</v>
       </c>
       <c r="I32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3712653778558872</v>
       </c>
       <c r="K32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.0264005151320021</v>
       </c>
       <c r="L32">
@@ -2174,13 +2171,13 @@
         <v>1.0001853224610822</v>
       </c>
       <c r="M32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="B33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
       <c r="C33" s="4">
@@ -2196,19 +2193,19 @@
         <v>45.06</v>
       </c>
       <c r="G33">
-        <f>C33/D33</f>
+        <f t="shared" si="4"/>
         <v>8.7265952491849088</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>20.790057700843317</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3823790501553481</v>
       </c>
       <c r="K33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.0415584415584416</v>
       </c>
       <c r="L33">
@@ -2216,7 +2213,7 @@
         <v>1.000093161915409</v>
       </c>
       <c r="M33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2226,7 +2223,7 @@
         <v>int</v>
       </c>
       <c r="B34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="C34" s="4">
@@ -2242,21 +2239,21 @@
         <v>6.04</v>
       </c>
       <c r="G34">
-        <f>C34/D34</f>
+        <f t="shared" si="4"/>
         <v>3.0467571644042231</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.6887417218543046</v>
       </c>
       <c r="I34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.1953642384105958</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="B35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="C35" s="4">
@@ -2272,21 +2269,21 @@
         <v>11.61</v>
       </c>
       <c r="G35">
-        <f>C35/D35</f>
+        <f t="shared" si="4"/>
         <v>3.0308404009252121</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.7717484926787259</v>
       </c>
       <c r="I35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.2342807924203276</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="B36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="C36" s="4">
@@ -2302,21 +2299,21 @@
         <v>22.76</v>
       </c>
       <c r="G36">
-        <f>C36/D36</f>
+        <f t="shared" si="4"/>
         <v>2.8780578206078578</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.8233743409490337</v>
       </c>
       <c r="I36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3708260105448153</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="B37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
       <c r="C37" s="4">
@@ -2332,15 +2329,15 @@
         <v>45.06</v>
       </c>
       <c r="G37">
-        <f>C37/D37</f>
+        <f t="shared" si="4"/>
         <v>2.8693869945966086</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.8353306702174876</v>
       </c>
       <c r="I37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3821571238348866</v>
       </c>
     </row>
@@ -2365,17 +2362,17 @@
   <sheetData>
     <row r="2" spans="2:20">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:20">
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:20">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:20">
@@ -2922,17 +2919,17 @@
   <sheetData>
     <row r="2" spans="2:15">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -3273,22 +3270,22 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -3298,7 +3295,7 @@
     </row>
     <row r="8" spans="2:6">
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add Results for Due
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Arduino Uno" sheetId="4" r:id="rId2"/>
     <sheet name="Arduino M0 Pro" sheetId="1" r:id="rId3"/>
     <sheet name="Maple" sheetId="5" r:id="rId4"/>
+    <sheet name="Arduino Due" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>Float</t>
   </si>
@@ -88,9 +89,6 @@
     <t>Sample Rate</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>usec</t>
   </si>
   <si>
@@ -150,13 +148,32 @@
   <si>
     <t>16 MHz</t>
   </si>
+  <si>
+    <t>Arduino Due</t>
+  </si>
+  <si>
+    <t>https://www.arduino.cc/en/Main/arduinoBoardDue</t>
+  </si>
+  <si>
+    <t>Atmel SAM3X8E ARM Cortex-M3 CPU</t>
+  </si>
+  <si>
+    <t>84 MHz</t>
+  </si>
+  <si>
+    <t>Uno/Due</t>
+  </si>
+  <si>
+    <t>Maple/Due</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -199,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -208,13 +225,162 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -237,6 +403,33 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filtering (in</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> C, f</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>loat)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -244,10 +437,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11423840769903762"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.75980227471566053"/>
-          <c:h val="0.8326195683872849"/>
+          <c:x val="0.15304642013303429"/>
+          <c:y val="0.16714129483814524"/>
+          <c:w val="0.76257425202307094"/>
+          <c:h val="0.67521216097987746"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -267,15 +460,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Comparison!$B$5:$B$10</c:f>
@@ -346,21 +530,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Comparison!$B$5:$B$13</c:f>
+              <c:f>Comparison!$B$5:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -384,19 +559,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Comparison!$D$5:$D$13</c:f>
+              <c:f>Comparison!$D$5:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>30.2</c:v>
                 </c:pt>
@@ -421,8 +593,164 @@
                 <c:pt idx="7">
                   <c:v>3761</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>7519</c:v>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Maple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$E$6:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>154.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>310.14999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>620.58000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1241.3699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$F$6:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>17.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>143.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>286.93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>573.83000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1147.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,28 +765,48 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104930304"/>
-        <c:axId val="104936192"/>
+        <c:axId val="133241472"/>
+        <c:axId val="131895680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104930304"/>
+        <c:axId val="133241472"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="1100"/>
+          <c:max val="512"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FIR Filter Length</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104936192"/>
+        <c:crossAx val="131895680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104936192"/>
+        <c:axId val="131895680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -467,11 +815,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to Complete (microseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104930304"/>
+        <c:crossAx val="133241472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -482,13 +849,25 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.59536001749781275"/>
-          <c:y val="0.59683836395450574"/>
-          <c:w val="0.36426552930883638"/>
-          <c:h val="0.26890237678623508"/>
+          <c:x val="0.63971210459399441"/>
+          <c:y val="0.58155237647782076"/>
+          <c:w val="0.27556152154577351"/>
+          <c:h val="0.22609889054336346"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -812,11 +1191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104961920"/>
-        <c:axId val="104963456"/>
+        <c:axId val="44090496"/>
+        <c:axId val="44092032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104961920"/>
+        <c:axId val="44090496"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -829,12 +1208,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104963456"/>
+        <c:crossAx val="44092032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104963456"/>
+        <c:axId val="44092032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -846,9 +1225,596 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104961920"/>
+        <c:crossAx val="44090496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filtering Performance (in C)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$27:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>549.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>224.49</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>77.28</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>71.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>long</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$31:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>236.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.94</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$35:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.94</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="133849856"/>
+        <c:axId val="133851392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="133849856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133851392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133851392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time for 32-Point FIR (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133849856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filtering Performance (in C)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$27:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>549.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>224.49</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>77.28</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>71.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>long</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$31:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>236.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.94</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Maple</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$C$35:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.94</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="134016000"/>
+        <c:axId val="149234432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="134016000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149234432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149234432"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time for 64-Point FIR (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134016000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -872,16 +1838,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -902,13 +1868,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
@@ -925,6 +1891,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1092,6 +2120,66 @@
         <a:xfrm>
           <a:off x="4371975" y="200025"/>
           <a:ext cx="2286000" cy="2181225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>13484</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://www.arduino.cc/en/uploads/Main/ArduinoDue_Front_450px.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4280684" y="828675"/>
+          <a:ext cx="4120365" cy="2200275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,23 +2488,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" customWidth="1"/>
-    <col min="7" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="2.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" customWidth="1"/>
+    <col min="8" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" customWidth="1"/>
+    <col min="12" max="13" width="9.28515625" customWidth="1"/>
+    <col min="14" max="14" width="2.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:9">
       <c r="C1" t="str">
         <f>'Arduino Uno'!I5</f>
         <v>Arduino Uno</v>
@@ -1426,13 +2516,14 @@
         <v>Arduino M0 Pro</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11">
+        <v>29</v>
+      </c>
+      <c r="F1" t="str">
+        <f>'Arduino Due'!C6</f>
+        <v>Arduino Due</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
       <c r="C2" t="str">
         <f>'Arduino Uno'!I6</f>
         <v>float</v>
@@ -1444,8 +2535,12 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
+      <c r="F2" t="str">
+        <f>'Arduino Due'!D8</f>
+        <v>float</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="C3" t="str">
         <f>'Arduino Uno'!I7</f>
         <v>function</v>
@@ -1457,31 +2552,35 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="F3" t="str">
+        <f>'Arduino Due'!C7</f>
+        <v>Inline, using types.h</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11">
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5">
         <f>'Arduino M0 Pro'!B10</f>
         <v>4</v>
@@ -1498,20 +2597,20 @@
         <f>Maple!D9</f>
         <v>9.26</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G10" si="0">C5/D5</f>
+      <c r="F5">
+        <f>'Arduino Due'!D9</f>
+        <v>8.61</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H10" si="0">C5/D5</f>
         <v>2.632450331125828</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>C5/E5</f>
         <v>8.5853131749460037</v>
       </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K12" si="1">D5/E5</f>
-        <v>3.2613390928725701</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6">
         <f>'Arduino M0 Pro'!B11</f>
         <v>8</v>
@@ -1528,20 +2627,20 @@
         <f>Maple!D10</f>
         <v>19</v>
       </c>
-      <c r="G6">
+      <c r="F6">
+        <f>'Arduino Due'!D10</f>
+        <v>17.670000000000002</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>2.6076884337753903</v>
       </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H10" si="2">C6/E6</f>
+      <c r="I6">
+        <f t="shared" ref="I6:I10" si="1">C6/E6</f>
         <v>8.1757894736842101</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>3.135263157894737</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7">
         <f>'Arduino M0 Pro'!B12</f>
         <v>16</v>
@@ -1558,20 +2657,20 @@
         <f>Maple!D11</f>
         <v>38.44</v>
       </c>
-      <c r="G7">
+      <c r="F7">
+        <f>'Arduino Due'!D11</f>
+        <v>35.69</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>2.6091293322062556</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
+      <c r="I7">
+        <f t="shared" si="1"/>
         <v>8.0296566077003124</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>3.0775234131113423</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8">
         <f>'Arduino M0 Pro'!B13</f>
         <v>32</v>
@@ -1588,20 +2687,20 @@
         <f>Maple!D12</f>
         <v>77.28</v>
       </c>
-      <c r="G8">
+      <c r="F8">
+        <f>'Arduino Due'!D12</f>
+        <v>71.64</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>2.6716595744680851</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
+      <c r="I8">
+        <f t="shared" si="1"/>
         <v>8.1242236024844718</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>3.0408902691511388</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9">
         <f>'Arduino M0 Pro'!B14</f>
         <v>64</v>
@@ -1618,20 +2717,20 @@
         <f>Maple!D13</f>
         <v>154.91999999999999</v>
       </c>
-      <c r="G9">
+      <c r="F9">
+        <f>'Arduino Due'!D13</f>
+        <v>143.43</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>2.7124735729386891</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
+      <c r="I9">
+        <f t="shared" si="1"/>
         <v>8.2816937774335155</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>3.0531887425768143</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10">
         <f>'Arduino M0 Pro'!B15</f>
         <v>128</v>
@@ -1648,20 +2747,20 @@
         <f>Maple!D14</f>
         <v>310.14999999999998</v>
       </c>
-      <c r="G10">
+      <c r="F10">
+        <f>'Arduino Due'!D14</f>
+        <v>286.93</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>2.7798941798941801</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
+      <c r="I10">
+        <f t="shared" si="1"/>
         <v>8.4700951152668065</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>3.0469127841367083</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11">
         <f>'Arduino M0 Pro'!B16</f>
         <v>256</v>
@@ -1678,12 +2777,12 @@
         <f>Maple!D15</f>
         <v>620.58000000000004</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>3.0407038576815237</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="F11">
+        <f>'Arduino Due'!D15</f>
+        <v>573.83000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12">
         <f>'Arduino M0 Pro'!B17</f>
         <v>512</v>
@@ -1700,12 +2799,12 @@
         <f>Maple!D16</f>
         <v>1241.3699999999999</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>3.0297171673231995</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="F12">
+        <f>'Arduino Due'!D16</f>
+        <v>1147.53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13">
         <f>'Arduino M0 Pro'!B18</f>
         <v>1024</v>
@@ -1719,7 +2818,7 @@
         <v>7519</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:9">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -1727,15 +2826,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:9">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="C17">
         <v>6000</v>
       </c>
@@ -1744,30 +2843,30 @@
         <v>166.66666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:18">
       <c r="C18">
         <v>8000</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" ref="D18:D21" si="3">1/C18*1000000</f>
+        <f t="shared" ref="D18:D21" si="2">1/C18*1000000</f>
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:18">
       <c r="C19">
         <v>11025</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>90.702947845804985</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:18">
       <c r="C20">
         <v>22050</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45.351473922902493</v>
       </c>
       <c r="E20" s="4"/>
@@ -1777,13 +2876,17 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="C21">
         <v>44100</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>22.675736961451246</v>
       </c>
       <c r="E21" s="4"/>
@@ -1793,8 +2896,12 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="C23" t="str">
         <f>'Arduino Uno'!L5</f>
         <v>Arduino Uno</v>
@@ -1804,34 +2911,50 @@
         <v>Arduino M0 Pro</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23">
+        <v>29</v>
+      </c>
+      <c r="F23" t="str">
+        <f>'Arduino Due'!C6</f>
+        <v>Arduino Due</v>
+      </c>
+      <c r="H23">
         <f>48/16</f>
         <v>3</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f>72/16</f>
         <v>4.5</v>
       </c>
-      <c r="I23">
+      <c r="J23">
+        <f>84/16</f>
+        <v>5.25</v>
+      </c>
+      <c r="L23">
         <f>72/48</f>
         <v>1.5</v>
       </c>
-      <c r="K23" t="str">
+      <c r="M23">
+        <f>84/72</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="O23" t="str">
         <f>C23</f>
         <v>Arduino Uno</v>
       </c>
-      <c r="L23" t="str">
+      <c r="P23" t="str">
         <f>D23</f>
         <v>Arduino M0 Pro</v>
       </c>
-      <c r="M23" t="str">
+      <c r="Q23" t="str">
         <f>E23</f>
         <v>Maple</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="R23" t="str">
+        <f>F23</f>
+        <v>Arduino Due</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="C24" t="str">
         <f>'Arduino Uno'!L6</f>
         <v>inline, using types.h</v>
@@ -1840,40 +2963,57 @@
         <f>'Arduino M0 Pro'!K7</f>
         <v>Inline, using types.h</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="E24" t="str">
+        <f>Maple!C7</f>
+        <v>Inline, using types.h</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="str">
+        <f>'Arduino Due'!C7</f>
+        <v>Inline, using types.h</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" t="s">
         <v>32</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L25" t="s">
         <v>33</v>
       </c>
-      <c r="I25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" t="s">
-        <v>29</v>
-      </c>
       <c r="M25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>48</v>
+      </c>
+      <c r="O25" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" t="str">
         <f>'Arduino Uno'!L7</f>
         <v>float</v>
@@ -1894,32 +3034,50 @@
         <f>Maple!D11</f>
         <v>38.44</v>
       </c>
-      <c r="G26">
-        <f t="shared" ref="G26:G37" si="4">C26/D26</f>
+      <c r="F26">
+        <f>'Arduino Due'!D11</f>
+        <v>35.69</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" ref="H26:H37" si="3">C26/D26</f>
         <v>2.3994661921708182</v>
       </c>
-      <c r="H26">
+      <c r="I26" s="6">
         <f>C26/E26</f>
         <v>7.0161290322580649</v>
       </c>
-      <c r="I26">
+      <c r="J26" s="6">
+        <f>C26/F26</f>
+        <v>7.556738582235921</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6">
         <f>D26/E26</f>
         <v>2.9240374609781479</v>
       </c>
-      <c r="K26">
+      <c r="M26" s="6">
+        <f>E26/F26</f>
+        <v>1.0770523956290277</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6">
         <f>C26/C34</f>
         <v>6.6757425742574261</v>
       </c>
-      <c r="L26">
+      <c r="P26" s="6">
         <f>D26/D34</f>
         <v>8.4766214177978885</v>
       </c>
-      <c r="M26">
+      <c r="Q26" s="6">
         <f>E26/E34</f>
         <v>6.3642384105960259</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="R26" s="6">
+        <f>F26/F34</f>
+        <v>5.499229583975346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="B27">
         <f>'Arduino Uno'!B12</f>
         <v>32</v>
@@ -1936,32 +3094,50 @@
         <f>Maple!D12</f>
         <v>77.28</v>
       </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
+      <c r="F27">
+        <f>'Arduino Due'!D12</f>
+        <v>71.64</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="3"/>
         <v>2.4459886854648314</v>
       </c>
-      <c r="H27">
-        <f t="shared" ref="H27:H37" si="5">C27/E27</f>
+      <c r="I27" s="6">
+        <f t="shared" ref="I27:I37" si="4">C27/E27</f>
         <v>7.1053312629399592</v>
       </c>
-      <c r="I27">
-        <f t="shared" ref="I27:I37" si="6">D27/E27</f>
+      <c r="J27" s="6">
+        <f t="shared" ref="J27:J37" si="5">C27/F27</f>
+        <v>7.6647124511446121</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6">
+        <f t="shared" ref="L27:L37" si="6">D27/E27</f>
         <v>2.9048913043478262</v>
       </c>
-      <c r="K27">
-        <f t="shared" ref="K27:K29" si="7">C27/C35</f>
+      <c r="M27" s="6">
+        <f t="shared" ref="M27:M37" si="7">E27/F27</f>
+        <v>1.0787269681742044</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6">
+        <f t="shared" ref="O27:O29" si="8">C27/C35</f>
         <v>6.9842279318239635</v>
       </c>
-      <c r="L27">
+      <c r="P27" s="6">
         <f>D27/D35</f>
         <v>8.6542020046260593</v>
       </c>
-      <c r="M27">
-        <f t="shared" ref="M27:M29" si="8">E27/E35</f>
+      <c r="Q27" s="6">
+        <f t="shared" ref="Q27:R29" si="9">E27/E35</f>
         <v>6.6563307493540051</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="R27" s="6">
+        <f t="shared" si="9"/>
+        <v>5.6857142857142859</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="B28">
         <f>'Arduino Uno'!B13</f>
         <v>64</v>
@@ -1978,32 +3154,50 @@
         <f>Maple!D13</f>
         <v>154.91999999999999</v>
       </c>
-      <c r="G28">
+      <c r="F28">
+        <f>'Arduino Due'!D13</f>
+        <v>143.43</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="3"/>
+        <v>2.4946388698516571</v>
+      </c>
+      <c r="I28" s="6">
         <f t="shared" si="4"/>
-        <v>2.4946388698516571</v>
-      </c>
-      <c r="H28">
+        <v>7.2837593596695083</v>
+      </c>
+      <c r="J28" s="6">
         <f t="shared" si="5"/>
-        <v>7.2837593596695083</v>
-      </c>
-      <c r="I28">
+        <v>7.8672523182040024</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6">
         <f t="shared" si="6"/>
         <v>2.9197650400206561</v>
       </c>
-      <c r="K28">
+      <c r="M28" s="6">
         <f t="shared" si="7"/>
+        <v>1.0801087638569336</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6">
+        <f t="shared" si="8"/>
         <v>7.2659368963296842</v>
       </c>
-      <c r="L28">
+      <c r="P28" s="6">
         <f>D28/D36</f>
         <v>8.3826908821349146</v>
       </c>
-      <c r="M28">
-        <f t="shared" si="8"/>
+      <c r="Q28" s="6">
+        <f t="shared" si="9"/>
         <v>6.8066783831282942</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="R28" s="6">
+        <f t="shared" si="9"/>
+        <v>5.7834677419354836</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="B29">
         <f>'Arduino Uno'!B14</f>
         <v>128</v>
@@ -2020,32 +3214,50 @@
         <f>Maple!D14</f>
         <v>310.14999999999998</v>
       </c>
-      <c r="G29">
+      <c r="F29">
+        <f>'Arduino Due'!D14</f>
+        <v>286.93</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="3"/>
+        <v>2.5816660764872523</v>
+      </c>
+      <c r="I29" s="6">
         <f t="shared" si="4"/>
-        <v>2.5816660764872523</v>
-      </c>
-      <c r="H29">
+        <v>7.5221666935353868</v>
+      </c>
+      <c r="J29" s="6">
         <f t="shared" si="5"/>
-        <v>7.5221666935353868</v>
-      </c>
-      <c r="I29">
+        <v>8.1309030077022264</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6">
         <f t="shared" si="6"/>
         <v>2.9136869256811222</v>
       </c>
-      <c r="K29">
+      <c r="M29" s="6">
         <f t="shared" si="7"/>
+        <v>1.0809256613111211</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6">
+        <f t="shared" si="8"/>
         <v>7.5746753246753249</v>
       </c>
-      <c r="L29">
+      <c r="P29" s="6">
         <f>D29/D37</f>
         <v>8.4188559716787772</v>
       </c>
-      <c r="M29">
-        <f t="shared" si="8"/>
+      <c r="Q29" s="6">
+        <f t="shared" si="9"/>
         <v>6.8830448291167325</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="R29" s="6">
+        <f t="shared" si="9"/>
+        <v>5.83072546230441</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" t="str">
         <f>'Arduino Uno'!N7</f>
         <v>long</v>
@@ -2066,34 +3278,52 @@
         <f>Maple!E11</f>
         <v>6.04</v>
       </c>
-      <c r="G30">
+      <c r="F30">
+        <f>'Arduino Due'!E11</f>
+        <v>6.49</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="3"/>
+        <v>9.0346907993966816</v>
+      </c>
+      <c r="I30" s="6">
         <f t="shared" si="4"/>
-        <v>9.0346907993966816</v>
-      </c>
-      <c r="H30">
+        <v>19.834437086092716</v>
+      </c>
+      <c r="J30" s="6">
         <f t="shared" si="5"/>
-        <v>19.834437086092716</v>
-      </c>
-      <c r="I30">
+        <v>18.459167950693374</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6">
         <f t="shared" si="6"/>
         <v>2.1953642384105958</v>
       </c>
-      <c r="K30">
+      <c r="M30" s="6">
+        <f t="shared" si="7"/>
+        <v>0.93066255778120177</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6">
         <f>C30/C34</f>
         <v>2.9653465346534653</v>
       </c>
-      <c r="L30">
+      <c r="P30" s="6">
         <f>D30/D34</f>
         <v>1</v>
       </c>
-      <c r="M30">
+      <c r="Q30" s="6">
         <f>E30/E34</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="R30" s="6">
+        <f>F30/F34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="B31">
-        <f t="shared" ref="B31:B37" si="9">B27</f>
+        <f t="shared" ref="B31:B37" si="10">B27</f>
         <v>32</v>
       </c>
       <c r="C31" s="4">
@@ -2108,34 +3338,52 @@
         <f>Maple!E12</f>
         <v>11.61</v>
       </c>
-      <c r="G31">
+      <c r="F31">
+        <f>'Arduino Due'!E12</f>
+        <v>12.6</v>
+      </c>
+      <c r="H31" s="6">
+        <f t="shared" si="3"/>
+        <v>9.1187355435620656</v>
+      </c>
+      <c r="I31" s="6">
         <f t="shared" si="4"/>
-        <v>9.1187355435620656</v>
-      </c>
-      <c r="H31">
+        <v>20.373815676141259</v>
+      </c>
+      <c r="J31" s="6">
         <f t="shared" si="5"/>
-        <v>20.373815676141259</v>
-      </c>
-      <c r="I31">
+        <v>18.773015873015872</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6">
         <f t="shared" si="6"/>
         <v>2.2342807924203276</v>
       </c>
-      <c r="K31">
-        <f t="shared" ref="K31:K33" si="10">C31/C35</f>
+      <c r="M31" s="6">
+        <f t="shared" si="7"/>
+        <v>0.92142857142857137</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6">
+        <f t="shared" ref="O31:O33" si="11">C31/C35</f>
         <v>3.0086491986771811</v>
       </c>
-      <c r="L31">
+      <c r="P31" s="6">
         <f>D31/D35</f>
         <v>1</v>
       </c>
-      <c r="M31">
-        <f t="shared" ref="M31:M33" si="11">E31/E35</f>
+      <c r="Q31" s="6">
+        <f t="shared" ref="Q31:R33" si="12">E31/E35</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="R31" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="B32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="C32" s="4">
@@ -2150,34 +3398,52 @@
         <f>Maple!E13</f>
         <v>22.76</v>
       </c>
-      <c r="G32">
+      <c r="F32">
+        <f>'Arduino Due'!E13</f>
+        <v>24.8</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="3"/>
+        <v>8.7085417824717446</v>
+      </c>
+      <c r="I32" s="6">
         <f t="shared" si="4"/>
-        <v>8.7085417824717446</v>
-      </c>
-      <c r="H32">
+        <v>20.650263620386642</v>
+      </c>
+      <c r="J32" s="6">
         <f t="shared" si="5"/>
-        <v>20.650263620386642</v>
-      </c>
-      <c r="I32">
+        <v>18.951612903225804</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6">
         <f t="shared" si="6"/>
         <v>2.3712653778558872</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="10"/>
+      <c r="M32" s="6">
+        <f t="shared" si="7"/>
+        <v>0.91774193548387095</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6">
+        <f t="shared" si="11"/>
         <v>3.0264005151320021</v>
       </c>
-      <c r="L32">
+      <c r="P32" s="6">
         <f>D32/D36</f>
         <v>1.0001853224610822</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="11"/>
+      <c r="Q32" s="6">
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="R32" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="B33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="C33" s="4">
@@ -2192,38 +3458,56 @@
         <f>Maple!E14</f>
         <v>45.06</v>
       </c>
-      <c r="G33">
+      <c r="F33">
+        <f>'Arduino Due'!E14</f>
+        <v>49.21</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="3"/>
+        <v>8.7265952491849088</v>
+      </c>
+      <c r="I33" s="6">
         <f t="shared" si="4"/>
-        <v>8.7265952491849088</v>
-      </c>
-      <c r="H33">
+        <v>20.790057700843317</v>
+      </c>
+      <c r="J33" s="6">
         <f t="shared" si="5"/>
-        <v>20.790057700843317</v>
-      </c>
-      <c r="I33">
+        <v>19.036781142044298</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6">
         <f t="shared" si="6"/>
         <v>2.3823790501553481</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="10"/>
+      <c r="M33" s="6">
+        <f t="shared" si="7"/>
+        <v>0.91566754724649468</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6">
+        <f t="shared" si="11"/>
         <v>3.0415584415584416</v>
       </c>
-      <c r="L33">
+      <c r="P33" s="6">
         <f>D33/D37</f>
         <v>1.000093161915409</v>
       </c>
-      <c r="M33">
-        <f t="shared" si="11"/>
+      <c r="Q33" s="6">
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="R33" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" t="str">
         <f>'Arduino Uno'!M7</f>
         <v>int</v>
       </c>
       <c r="B34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="C34" s="4">
@@ -2238,22 +3522,40 @@
         <f>Maple!F11</f>
         <v>6.04</v>
       </c>
-      <c r="G34">
+      <c r="F34">
+        <f>'Arduino Due'!F11</f>
+        <v>6.49</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="3"/>
+        <v>3.0467571644042231</v>
+      </c>
+      <c r="I34" s="6">
         <f t="shared" si="4"/>
-        <v>3.0467571644042231</v>
-      </c>
-      <c r="H34">
+        <v>6.6887417218543046</v>
+      </c>
+      <c r="J34" s="6">
         <f t="shared" si="5"/>
-        <v>6.6887417218543046</v>
-      </c>
-      <c r="I34">
+        <v>6.2249614791987673</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6">
         <f t="shared" si="6"/>
         <v>2.1953642384105958</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="M34" s="6">
+        <f t="shared" si="7"/>
+        <v>0.93066255778120177</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="B35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="C35" s="4">
@@ -2268,22 +3570,40 @@
         <f>Maple!F12</f>
         <v>11.61</v>
       </c>
-      <c r="G35">
+      <c r="F35">
+        <f>'Arduino Due'!F12</f>
+        <v>12.6</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="3"/>
+        <v>3.0308404009252121</v>
+      </c>
+      <c r="I35" s="6">
         <f t="shared" si="4"/>
-        <v>3.0308404009252121</v>
-      </c>
-      <c r="H35">
+        <v>6.7717484926787259</v>
+      </c>
+      <c r="J35" s="6">
         <f t="shared" si="5"/>
-        <v>6.7717484926787259</v>
-      </c>
-      <c r="I35">
+        <v>6.2396825396825406</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6">
         <f t="shared" si="6"/>
         <v>2.2342807924203276</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="M35" s="6">
+        <f t="shared" si="7"/>
+        <v>0.92142857142857137</v>
+      </c>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="B36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="C36" s="4">
@@ -2298,22 +3618,40 @@
         <f>Maple!F13</f>
         <v>22.76</v>
       </c>
-      <c r="G36">
+      <c r="F36">
+        <f>'Arduino Due'!F13</f>
+        <v>24.8</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="3"/>
+        <v>2.8780578206078578</v>
+      </c>
+      <c r="I36" s="6">
         <f t="shared" si="4"/>
-        <v>2.8780578206078578</v>
-      </c>
-      <c r="H36">
+        <v>6.8233743409490337</v>
+      </c>
+      <c r="J36" s="6">
         <f t="shared" si="5"/>
-        <v>6.8233743409490337</v>
-      </c>
-      <c r="I36">
+        <v>6.2620967741935489</v>
+      </c>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6">
         <f t="shared" si="6"/>
         <v>2.3708260105448153</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="M36" s="6">
+        <f t="shared" si="7"/>
+        <v>0.91774193548387095</v>
+      </c>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+    </row>
+    <row r="37" spans="1:18">
       <c r="B37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="C37" s="4">
@@ -2328,20 +3666,55 @@
         <f>Maple!F14</f>
         <v>45.06</v>
       </c>
-      <c r="G37">
+      <c r="F37">
+        <f>'Arduino Due'!F14</f>
+        <v>49.21</v>
+      </c>
+      <c r="H37" s="6">
+        <f t="shared" si="3"/>
+        <v>2.8693869945966086</v>
+      </c>
+      <c r="I37" s="6">
         <f t="shared" si="4"/>
-        <v>2.8693869945966086</v>
-      </c>
-      <c r="H37">
+        <v>6.8353306702174876</v>
+      </c>
+      <c r="J37" s="6">
         <f t="shared" si="5"/>
-        <v>6.8353306702174876</v>
-      </c>
-      <c r="I37">
+        <v>6.2588904694167855</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6">
         <f t="shared" si="6"/>
         <v>2.3821571238348866</v>
       </c>
+      <c r="M37" s="6">
+        <f t="shared" si="7"/>
+        <v>0.91566754724649468</v>
+      </c>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C26:F37">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="greaterThan">
+      <formula>$D$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>$D$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>$D$19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>$D$20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="lessThan">
+      <formula>$D$21</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2351,7 +3724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2362,17 +3735,17 @@
   <sheetData>
     <row r="2" spans="2:20">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:20">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:20">
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:20">
@@ -2388,7 +3761,7 @@
         <v>19</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:20">
@@ -2405,10 +3778,10 @@
         <v>19</v>
       </c>
       <c r="M7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" t="s">
         <v>26</v>
-      </c>
-      <c r="N7" t="s">
-        <v>27</v>
       </c>
       <c r="P7" t="s">
         <v>12</v>
@@ -2919,17 +4292,17 @@
   <sheetData>
     <row r="2" spans="2:15">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -2945,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -2962,10 +4335,10 @@
         <v>19</v>
       </c>
       <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
         <v>26</v>
-      </c>
-      <c r="M8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -3263,48 +4636,48 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -3441,6 +4814,197 @@
       </c>
       <c r="F16">
         <v>178.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>13.75</v>
+      </c>
+      <c r="D9">
+        <v>8.61</v>
+      </c>
+      <c r="E9">
+        <v>1.92</v>
+      </c>
+      <c r="F9">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>28.23</v>
+      </c>
+      <c r="D10">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="E10">
+        <v>3.44</v>
+      </c>
+      <c r="F10">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>57.06</v>
+      </c>
+      <c r="D11">
+        <v>35.69</v>
+      </c>
+      <c r="E11">
+        <v>6.49</v>
+      </c>
+      <c r="F11">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>114.59</v>
+      </c>
+      <c r="D12">
+        <v>71.64</v>
+      </c>
+      <c r="E12">
+        <v>12.6</v>
+      </c>
+      <c r="F12">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>229.52</v>
+      </c>
+      <c r="D13">
+        <v>143.43</v>
+      </c>
+      <c r="E13">
+        <v>24.8</v>
+      </c>
+      <c r="F13">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>459.25</v>
+      </c>
+      <c r="D14">
+        <v>286.93</v>
+      </c>
+      <c r="E14">
+        <v>49.21</v>
+      </c>
+      <c r="F14">
+        <v>49.21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>918.56</v>
+      </c>
+      <c r="D15">
+        <v>573.83000000000004</v>
+      </c>
+      <c r="E15">
+        <v>98.05</v>
+      </c>
+      <c r="F15">
+        <v>98.05</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16">
+        <v>512</v>
+      </c>
+      <c r="C16">
+        <v>1837.07</v>
+      </c>
+      <c r="D16">
+        <v>1147.53</v>
+      </c>
+      <c r="E16">
+        <v>195.67</v>
+      </c>
+      <c r="F16">
+        <v>195.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add results for Teensy 3.1
</commit_message>
<xml_diff>
--- a/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
+++ b/Arduino/2015-07_Benchmarking/FIR_Benchmarking/Speed Results.xlsx
@@ -12,13 +12,14 @@
     <sheet name="Arduino M0 Pro" sheetId="1" r:id="rId3"/>
     <sheet name="Maple" sheetId="5" r:id="rId4"/>
     <sheet name="Arduino Due" sheetId="6" r:id="rId5"/>
+    <sheet name="Teensy 3.1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
   <si>
     <t>Float</t>
   </si>
@@ -166,16 +167,63 @@
   <si>
     <t>Maple/Due</t>
   </si>
+  <si>
+    <t>96 MHz</t>
+  </si>
+  <si>
+    <t>96 MHz, Optimized</t>
+  </si>
+  <si>
+    <t>Teensy 3.1, 72MHz</t>
+  </si>
+  <si>
+    <t>72 MHz, Optimized</t>
+  </si>
+  <si>
+    <t>http://www.pjrc.com/teensy/teensy31.html</t>
+  </si>
+  <si>
+    <t>MK20DX256VLH7, Cortex-M4</t>
+  </si>
+  <si>
+    <t>Teensy 3.1</t>
+  </si>
+  <si>
+    <t>Uno/Teensy</t>
+  </si>
+  <si>
+    <t>Maple/Teensy</t>
+  </si>
+  <si>
+    <t>96 MHz, Not-Optimized</t>
+  </si>
+  <si>
+    <t>Relative to 96MHz, Optimized</t>
+  </si>
+  <si>
+    <t>fs for N=32</t>
+  </si>
+  <si>
+    <t>Sample Rate While Still Getting Required Resolution</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>Uno/Uno</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +241,12 @@
     <font>
       <sz val="10"/>
       <name val="Droid Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,11 +266,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -225,17 +280,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF33CC33"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -249,14 +322,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor rgb="FF33CC33"/>
         </patternFill>
       </fill>
     </dxf>
@@ -277,7 +343,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -291,7 +364,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -305,13 +385,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
@@ -319,56 +392,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -757,6 +781,82 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Teensy 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Comparison!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$G$6:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124.89</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>501.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1004.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -765,11 +865,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133241472"/>
-        <c:axId val="131895680"/>
+        <c:axId val="141344768"/>
+        <c:axId val="141346688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133241472"/>
+        <c:axId val="141344768"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -801,15 +901,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131895680"/>
+        <c:crossAx val="141346688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="131895680"/>
+        <c:axId val="141346688"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
           <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -838,9 +940,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133241472"/>
+        <c:crossAx val="141344768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="10"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -849,10 +953,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.63971210459399441"/>
-          <c:y val="0.58155237647782076"/>
-          <c:w val="0.27556152154577351"/>
-          <c:h val="0.22609889054336346"/>
+          <c:x val="0.69238015726204705"/>
+          <c:y val="0.48738438806648249"/>
+          <c:w val="0.26242659376517646"/>
+          <c:h val="0.32708209332000465"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1191,11 +1295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44090496"/>
-        <c:axId val="44092032"/>
+        <c:axId val="142178560"/>
+        <c:axId val="142180352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44090496"/>
+        <c:axId val="142178560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1208,12 +1312,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44092032"/>
+        <c:crossAx val="142180352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44092032"/>
+        <c:axId val="142180352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1225,7 +1329,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44090496"/>
+        <c:crossAx val="142178560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1304,9 +1408,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1318,16 +1422,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$27:$F$27</c:f>
+              <c:f>Comparison!$C$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>549.1</c:v>
                 </c:pt>
@@ -1339,6 +1446,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>71.64</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>62.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1361,9 +1471,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1375,16 +1485,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$31:$F$31</c:f>
+              <c:f>Comparison!$C$31:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>236.54</c:v>
                 </c:pt>
@@ -1396,6 +1509,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,9 +1534,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1432,16 +1548,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$35:$F$35</c:f>
+              <c:f>Comparison!$C$35:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>78.62</c:v>
                 </c:pt>
@@ -1453,6 +1572,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1467,11 +1589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133849856"/>
-        <c:axId val="133851392"/>
+        <c:axId val="141898880"/>
+        <c:axId val="141900416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133849856"/>
+        <c:axId val="141898880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,7 +1602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133851392"/>
+        <c:crossAx val="141900416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1488,7 +1610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133851392"/>
+        <c:axId val="141900416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133849856"/>
+        <c:crossAx val="141898880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1595,9 +1717,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1609,16 +1731,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$27:$F$27</c:f>
+              <c:f>Comparison!$C$27:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>549.1</c:v>
                 </c:pt>
@@ -1630,6 +1755,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>71.64</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>62.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,9 +1780,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1666,16 +1794,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$31:$F$31</c:f>
+              <c:f>Comparison!$C$31:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>236.54</c:v>
                 </c:pt>
@@ -1687,6 +1818,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,9 +1843,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Comparison!$C$23:$F$23</c:f>
+              <c:f>Comparison!$C$23:$G$23</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Arduino Uno</c:v>
                 </c:pt>
@@ -1723,16 +1857,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Teensy 3.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$35:$F$35</c:f>
+              <c:f>Comparison!$C$35:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>78.62</c:v>
                 </c:pt>
@@ -1744,6 +1881,9 @@
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1760,11 +1900,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134016000"/>
-        <c:axId val="149234432"/>
+        <c:axId val="141936896"/>
+        <c:axId val="141938688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134016000"/>
+        <c:axId val="141936896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149234432"/>
+        <c:crossAx val="141938688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1781,7 +1921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149234432"/>
+        <c:axId val="141938688"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1800,7 +1940,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time for 64-Point FIR (usec)</a:t>
+                  <a:t>Time for 32-Point FIR (usec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1812,7 +1952,557 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134016000"/>
+        <c:crossAx val="141936896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filtering Performance (in C)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21079662231946025"/>
+          <c:y val="0.19480351414406533"/>
+          <c:w val="0.64403785561582649"/>
+          <c:h val="0.6327117964421114"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Comparison!$C$60:$D$60,Comparison!$F$60:$G$60)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$C$61:$D$61,Comparison!$F$61:$G$61)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3765.5502941905706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5947.4704793272776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10561.849922156138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11318.689818636485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>long</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Comparison!$C$60:$D$60,Comparison!$F$60:$G$60)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$C$62:$D$62,Comparison!$F$62:$G$62)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5834.5996599157825</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17218.042770596836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25400.025400038103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46188.021535170061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="147399808"/>
+        <c:axId val="147403520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="147399808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147403520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="147403520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Max Sample Rate (Hz) For FIR with Resolution of 250 Hz</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.4282560706401765E-2"/>
+              <c:y val="0.16239610673665791"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147399808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10000"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FIR Filtering Performance (in C)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16542799327766317"/>
+          <c:y val="0.19480351414406533"/>
+          <c:w val="0.68940648465762355"/>
+          <c:h val="0.6327117964421114"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>int</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$I$41:$J$41,Comparison!$L$41:$M$41)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8780578206078578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2620967741935489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.706666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>long</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Comparison!$C$60:$D$60,Comparison!$F$60:$G$60)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$I$40:$J$40,Comparison!$L$40:$M$40)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.33042553191489366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8775245506763021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2620967741935489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.706666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Comparison!$C$60:$D$60,Comparison!$F$60:$G$60)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Uno</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Arduino M0 Pro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Arduino Due</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Comparison!$I$39:$J$39,Comparison!$L$39:$M$39)</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.13762850053172634</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34333340702584397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0827581398591648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2434942749619666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="147421440"/>
+        <c:axId val="147448576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="147421440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="147448576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="147448576"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speed Relative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to Uno (int)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.1843974784092163E-2"/>
+              <c:y val="0.20406277340332457"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147421440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,16 +2528,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1868,16 +2558,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1900,13 +2590,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1928,15 +2618,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1953,6 +2643,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514352</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2180,6 +2934,66 @@
         <a:xfrm>
           <a:off x="4280684" y="828675"/>
           <a:ext cx="4120365" cy="2200275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://www.pjrc.com/teensy/teensy31.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4257675" y="1038225"/>
+          <a:ext cx="3124200" cy="1762125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2488,25 +3302,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="P74" sqref="P74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="2.140625" customWidth="1"/>
-    <col min="8" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" customWidth="1"/>
-    <col min="12" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="2.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="4" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="13" width="9.28515625" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
+    <col min="15" max="17" width="9.28515625" customWidth="1"/>
+    <col min="18" max="18" width="2.5703125" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="2:13">
       <c r="C1" t="str">
         <f>'Arduino Uno'!I5</f>
         <v>Arduino Uno</v>
@@ -2522,8 +3337,11 @@
         <f>'Arduino Due'!C6</f>
         <v>Arduino Due</v>
       </c>
-    </row>
-    <row r="2" spans="2:9">
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13">
       <c r="C2" t="str">
         <f>'Arduino Uno'!I6</f>
         <v>float</v>
@@ -2539,8 +3357,11 @@
         <f>'Arduino Due'!D8</f>
         <v>float</v>
       </c>
-    </row>
-    <row r="3" spans="2:9">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
       <c r="C3" t="str">
         <f>'Arduino Uno'!I7</f>
         <v>function</v>
@@ -2556,8 +3377,12 @@
         <f>'Arduino Due'!C7</f>
         <v>Inline, using types.h</v>
       </c>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="G3" t="str">
+        <f>'Teensy 3.1'!C7</f>
+        <v>96 MHz, Optimized</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -2573,14 +3398,26 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5">
         <f>'Arduino M0 Pro'!B10</f>
         <v>4</v>
@@ -2601,16 +3438,32 @@
         <f>'Arduino Due'!D9</f>
         <v>8.61</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H10" si="0">C5/D5</f>
+      <c r="G5">
+        <f>'Teensy 3.1'!D9</f>
+        <v>6.81</v>
+      </c>
+      <c r="I5">
+        <f>C5/C5</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>C5/D5</f>
         <v>2.632450331125828</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f>C5/E5</f>
         <v>8.5853131749460037</v>
       </c>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="L5">
+        <f>$C5/F5</f>
+        <v>9.2334494773519165</v>
+      </c>
+      <c r="M5">
+        <f>$C5/G5</f>
+        <v>11.674008810572689</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6">
         <f>'Arduino M0 Pro'!B11</f>
         <v>8</v>
@@ -2631,16 +3484,32 @@
         <f>'Arduino Due'!D10</f>
         <v>17.670000000000002</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="G6">
+        <f>'Teensy 3.1'!D10</f>
+        <v>14.74</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I10" si="0">C6/C6</f>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>C6/D6</f>
         <v>2.6076884337753903</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I10" si="1">C6/E6</f>
+      <c r="K6">
+        <f>C6/E6</f>
         <v>8.1757894736842101</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="L6">
+        <f>$C6/F6</f>
+        <v>8.7911714770797964</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M10" si="1">$C6/G6</f>
+        <v>10.538670284938942</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7">
         <f>'Arduino M0 Pro'!B12</f>
         <v>16</v>
@@ -2661,16 +3530,32 @@
         <f>'Arduino Due'!D11</f>
         <v>35.69</v>
       </c>
-      <c r="H7">
+      <c r="G7">
+        <f>'Teensy 3.1'!D11</f>
+        <v>30.53</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f>C7/D7</f>
         <v>2.6091293322062556</v>
       </c>
-      <c r="I7">
+      <c r="K7">
+        <f>C7/E7</f>
+        <v>8.0296566077003124</v>
+      </c>
+      <c r="L7">
+        <f>$C7/F7</f>
+        <v>8.6483608854020755</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="1"/>
-        <v>8.0296566077003124</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
+        <v>10.110055682934819</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8">
         <f>'Arduino M0 Pro'!B13</f>
         <v>32</v>
@@ -2691,16 +3576,32 @@
         <f>'Arduino Due'!D12</f>
         <v>71.64</v>
       </c>
-      <c r="H8">
+      <c r="G8">
+        <f>'Teensy 3.1'!D12</f>
+        <v>62.01</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>C8/D8</f>
         <v>2.6716595744680851</v>
       </c>
-      <c r="I8">
+      <c r="K8">
+        <f>C8/E8</f>
+        <v>8.1242236024844718</v>
+      </c>
+      <c r="L8">
+        <f>$C8/F8</f>
+        <v>8.7638190954773876</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="1"/>
-        <v>8.1242236024844718</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
+        <v>10.124818577648767</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9">
         <f>'Arduino M0 Pro'!B14</f>
         <v>64</v>
@@ -2721,16 +3622,32 @@
         <f>'Arduino Due'!D13</f>
         <v>143.43</v>
       </c>
-      <c r="H9">
+      <c r="G9">
+        <f>'Teensy 3.1'!D13</f>
+        <v>124.89</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>C9/D9</f>
         <v>2.7124735729386891</v>
       </c>
-      <c r="I9">
+      <c r="K9">
+        <f>C9/E9</f>
+        <v>8.2816937774335155</v>
+      </c>
+      <c r="L9">
+        <f>$C9/F9</f>
+        <v>8.945130028585373</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="1"/>
-        <v>8.2816937774335155</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
+        <v>10.273040275442389</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
       <c r="B10">
         <f>'Arduino M0 Pro'!B15</f>
         <v>128</v>
@@ -2751,16 +3668,32 @@
         <f>'Arduino Due'!D14</f>
         <v>286.93</v>
       </c>
-      <c r="H10">
+      <c r="G10">
+        <f>'Teensy 3.1'!D14</f>
+        <v>250.57</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>C10/D10</f>
         <v>2.7798941798941801</v>
       </c>
-      <c r="I10">
+      <c r="K10">
+        <f>C10/E10</f>
+        <v>8.4700951152668065</v>
+      </c>
+      <c r="L10">
+        <f>$C10/F10</f>
+        <v>9.1555431638378693</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="1"/>
-        <v>8.4700951152668065</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
+        <v>10.484096260526002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11">
         <f>'Arduino M0 Pro'!B16</f>
         <v>256</v>
@@ -2781,8 +3714,12 @@
         <f>'Arduino Due'!D15</f>
         <v>573.83000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="G11">
+        <f>'Teensy 3.1'!D15</f>
+        <v>501.85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12">
         <f>'Arduino M0 Pro'!B17</f>
         <v>512</v>
@@ -2803,8 +3740,12 @@
         <f>'Arduino Due'!D16</f>
         <v>1147.53</v>
       </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="G12">
+        <f>'Teensy 3.1'!D16</f>
+        <v>1004.33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13">
         <f>'Arduino M0 Pro'!B18</f>
         <v>1024</v>
@@ -2818,7 +3759,7 @@
         <v>7519</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:13">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -2826,7 +3767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:13">
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -2834,7 +3775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:23">
       <c r="C17">
         <v>6000</v>
       </c>
@@ -2843,7 +3784,7 @@
         <v>166.66666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:23">
       <c r="C18">
         <v>8000</v>
       </c>
@@ -2852,7 +3793,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:23">
       <c r="C19">
         <v>11025</v>
       </c>
@@ -2861,7 +3802,7 @@
         <v>90.702947845804985</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:23">
       <c r="C20">
         <v>22050</v>
       </c>
@@ -2880,8 +3821,12 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="C21">
         <v>44100</v>
       </c>
@@ -2900,8 +3845,12 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="23" spans="1:23">
       <c r="C23" t="str">
         <f>'Arduino Uno'!L5</f>
         <v>Arduino Uno</v>
@@ -2917,44 +3866,60 @@
         <f>'Arduino Due'!C6</f>
         <v>Arduino Due</v>
       </c>
-      <c r="H23">
+      <c r="G23" t="str">
+        <f>'Teensy 3.1'!C6</f>
+        <v>Teensy 3.1</v>
+      </c>
+      <c r="J23">
         <f>48/16</f>
         <v>3</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <f>72/16</f>
         <v>4.5</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <f>84/16</f>
         <v>5.25</v>
       </c>
-      <c r="L23">
+      <c r="M23">
+        <f>96/16</f>
+        <v>6</v>
+      </c>
+      <c r="O23">
         <f>72/48</f>
         <v>1.5</v>
       </c>
-      <c r="M23">
+      <c r="P23">
         <f>84/72</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="O23" t="str">
+      <c r="Q23">
+        <f>96/72</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="S23" t="str">
         <f>C23</f>
         <v>Arduino Uno</v>
       </c>
-      <c r="P23" t="str">
+      <c r="T23" t="str">
         <f>D23</f>
         <v>Arduino M0 Pro</v>
       </c>
-      <c r="Q23" t="str">
+      <c r="U23" t="str">
         <f>E23</f>
         <v>Maple</v>
       </c>
-      <c r="R23" t="str">
+      <c r="V23" t="str">
         <f>F23</f>
         <v>Arduino Due</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="W23" t="str">
+        <f>G23</f>
+        <v>Teensy 3.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="C24" t="str">
         <f>'Arduino Uno'!L6</f>
         <v>inline, using types.h</v>
@@ -2967,8 +3932,12 @@
         <f>Maple!C7</f>
         <v>Inline, using types.h</v>
       </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="G24" t="str">
+        <f>'Teensy 3.1'!C7</f>
+        <v>96 MHz, Optimized</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="B25" t="s">
         <v>2</v>
       </c>
@@ -2981,39 +3950,53 @@
       <c r="E25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" t="str">
-        <f>'Arduino Due'!C7</f>
-        <v>Inline, using types.h</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" t="s">
         <v>31</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>32</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
         <v>47</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" t="s">
         <v>33</v>
       </c>
-      <c r="M25" t="s">
+      <c r="P25" t="s">
         <v>48</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
+        <v>57</v>
+      </c>
+      <c r="S25" t="s">
         <v>28</v>
       </c>
-      <c r="P25" t="s">
+      <c r="T25" t="s">
         <v>28</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="U25" t="s">
         <v>28</v>
       </c>
-      <c r="R25" t="s">
+      <c r="V25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="W25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="str">
         <f>'Arduino Uno'!L7</f>
         <v>float</v>
@@ -3038,46 +4021,66 @@
         <f>'Arduino Due'!D11</f>
         <v>35.69</v>
       </c>
-      <c r="H26" s="6">
-        <f t="shared" ref="H26:H37" si="3">C26/D26</f>
+      <c r="G26">
+        <f>'Teensy 3.1'!D11</f>
+        <v>30.53</v>
+      </c>
+      <c r="I26">
+        <f>C26/C26</f>
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
+        <f>C26/D26</f>
         <v>2.3994661921708182</v>
       </c>
-      <c r="I26" s="6">
+      <c r="K26" s="6">
         <f>C26/E26</f>
         <v>7.0161290322580649</v>
       </c>
-      <c r="J26" s="6">
-        <f>C26/F26</f>
+      <c r="L26" s="6">
+        <f>$C26/F26</f>
         <v>7.556738582235921</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6">
+      <c r="M26" s="6">
+        <f>$C26/G26</f>
+        <v>8.8339338355715675</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6">
         <f>D26/E26</f>
         <v>2.9240374609781479</v>
       </c>
-      <c r="M26" s="6">
+      <c r="P26" s="6">
         <f>E26/F26</f>
         <v>1.0770523956290277</v>
       </c>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6">
+      <c r="Q26" s="6">
+        <f>E26/G26</f>
+        <v>1.2590894202423843</v>
+      </c>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6">
         <f>C26/C34</f>
         <v>6.6757425742574261</v>
       </c>
-      <c r="P26" s="6">
+      <c r="T26" s="6">
         <f>D26/D34</f>
         <v>8.4766214177978885</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="U26" s="6">
         <f>E26/E34</f>
         <v>6.3642384105960259</v>
       </c>
-      <c r="R26" s="6">
+      <c r="V26" s="6">
         <f>F26/F34</f>
         <v>5.499229583975346</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="W26" s="6">
+        <f>G26/G34</f>
+        <v>15.341708542713569</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="B27">
         <f>'Arduino Uno'!B12</f>
         <v>32</v>
@@ -3098,46 +4101,66 @@
         <f>'Arduino Due'!D12</f>
         <v>71.64</v>
       </c>
-      <c r="H27" s="6">
-        <f t="shared" si="3"/>
+      <c r="G27">
+        <f>'Teensy 3.1'!D12</f>
+        <v>62.01</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I37" si="3">C27/C27</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="6">
+        <f>C27/D27</f>
         <v>2.4459886854648314</v>
       </c>
-      <c r="I27" s="6">
-        <f t="shared" ref="I27:I37" si="4">C27/E27</f>
+      <c r="K27" s="6">
+        <f>C27/E27</f>
         <v>7.1053312629399592</v>
       </c>
-      <c r="J27" s="6">
-        <f t="shared" ref="J27:J37" si="5">C27/F27</f>
+      <c r="L27" s="6">
+        <f>$C27/F27</f>
         <v>7.6647124511446121</v>
       </c>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6">
-        <f t="shared" ref="L27:L37" si="6">D27/E27</f>
-        <v>2.9048913043478262</v>
-      </c>
       <c r="M27" s="6">
-        <f t="shared" ref="M27:M37" si="7">E27/F27</f>
-        <v>1.0787269681742044</v>
+        <f t="shared" ref="M27:M37" si="4">$C27/G27</f>
+        <v>8.8550233833252712</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6">
-        <f t="shared" ref="O27:O29" si="8">C27/C35</f>
+        <f>D27/E27</f>
+        <v>2.9048913043478262</v>
+      </c>
+      <c r="P27" s="6">
+        <f>E27/F27</f>
+        <v>1.0787269681742044</v>
+      </c>
+      <c r="Q27" s="6">
+        <f>E27/G27</f>
+        <v>1.2462506047411708</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6">
+        <f>C27/C35</f>
         <v>6.9842279318239635</v>
       </c>
-      <c r="P27" s="6">
+      <c r="T27" s="6">
         <f>D27/D35</f>
         <v>8.6542020046260593</v>
       </c>
-      <c r="Q27" s="6">
-        <f t="shared" ref="Q27:R29" si="9">E27/E35</f>
+      <c r="U27" s="6">
+        <f>E27/E35</f>
         <v>6.6563307493540051</v>
       </c>
-      <c r="R27" s="6">
-        <f t="shared" si="9"/>
+      <c r="V27" s="6">
+        <f>F27/F35</f>
         <v>5.6857142857142859</v>
       </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="W27" s="6">
+        <f t="shared" ref="W27:W29" si="5">G27/G35</f>
+        <v>16.232984293193716</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="B28">
         <f>'Arduino Uno'!B13</f>
         <v>64</v>
@@ -3158,46 +4181,66 @@
         <f>'Arduino Due'!D13</f>
         <v>143.43</v>
       </c>
-      <c r="H28" s="6">
+      <c r="G28">
+        <f>'Teensy 3.1'!D13</f>
+        <v>124.89</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="6">
+        <f>C28/D28</f>
         <v>2.4946388698516571</v>
       </c>
-      <c r="I28" s="6">
+      <c r="K28" s="6">
+        <f>C28/E28</f>
+        <v>7.2837593596695083</v>
+      </c>
+      <c r="L28" s="6">
+        <f>$C28/F28</f>
+        <v>7.8672523182040024</v>
+      </c>
+      <c r="M28" s="6">
         <f t="shared" si="4"/>
-        <v>7.2837593596695083</v>
-      </c>
-      <c r="J28" s="6">
-        <f t="shared" si="5"/>
-        <v>7.8672523182040024</v>
-      </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6">
-        <f t="shared" si="6"/>
-        <v>2.9197650400206561</v>
-      </c>
-      <c r="M28" s="6">
-        <f t="shared" si="7"/>
-        <v>1.0801087638569336</v>
+        <v>9.0351509328208834</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6">
-        <f t="shared" si="8"/>
+        <f>D28/E28</f>
+        <v>2.9197650400206561</v>
+      </c>
+      <c r="P28" s="6">
+        <f>E28/F28</f>
+        <v>1.0801087638569336</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>E28/G28</f>
+        <v>1.2404515974057169</v>
+      </c>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6">
+        <f>C28/C36</f>
         <v>7.2659368963296842</v>
       </c>
-      <c r="P28" s="6">
+      <c r="T28" s="6">
         <f>D28/D36</f>
         <v>8.3826908821349146</v>
       </c>
-      <c r="Q28" s="6">
-        <f t="shared" si="9"/>
+      <c r="U28" s="6">
+        <f>E28/E36</f>
         <v>6.8066783831282942</v>
       </c>
-      <c r="R28" s="6">
-        <f t="shared" si="9"/>
+      <c r="V28" s="6">
+        <f>F28/F36</f>
         <v>5.7834677419354836</v>
       </c>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="W28" s="6">
+        <f t="shared" si="5"/>
+        <v>16.652000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="B29">
         <f>'Arduino Uno'!B14</f>
         <v>128</v>
@@ -3218,46 +4261,66 @@
         <f>'Arduino Due'!D14</f>
         <v>286.93</v>
       </c>
-      <c r="H29" s="6">
+      <c r="G29">
+        <f>'Teensy 3.1'!D14</f>
+        <v>250.57</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
+        <f>C29/D29</f>
         <v>2.5816660764872523</v>
       </c>
-      <c r="I29" s="6">
+      <c r="K29" s="6">
+        <f>C29/E29</f>
+        <v>7.5221666935353868</v>
+      </c>
+      <c r="L29" s="6">
+        <f>$C29/F29</f>
+        <v>8.1309030077022264</v>
+      </c>
+      <c r="M29" s="6">
         <f t="shared" si="4"/>
-        <v>7.5221666935353868</v>
-      </c>
-      <c r="J29" s="6">
-        <f t="shared" si="5"/>
-        <v>8.1309030077022264</v>
-      </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6">
-        <f t="shared" si="6"/>
-        <v>2.9136869256811222</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="7"/>
-        <v>1.0809256613111211</v>
+        <v>9.3107714411142606</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6">
-        <f t="shared" si="8"/>
+        <f>D29/E29</f>
+        <v>2.9136869256811222</v>
+      </c>
+      <c r="P29" s="6">
+        <f>E29/F29</f>
+        <v>1.0809256613111211</v>
+      </c>
+      <c r="Q29" s="6">
+        <f>E29/G29</f>
+        <v>1.237777866464461</v>
+      </c>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6">
+        <f>C29/C37</f>
         <v>7.5746753246753249</v>
       </c>
-      <c r="P29" s="6">
+      <c r="T29" s="6">
         <f>D29/D37</f>
         <v>8.4188559716787772</v>
       </c>
-      <c r="Q29" s="6">
-        <f t="shared" si="9"/>
+      <c r="U29" s="6">
+        <f>E29/E37</f>
         <v>6.8830448291167325</v>
       </c>
-      <c r="R29" s="6">
-        <f t="shared" si="9"/>
+      <c r="V29" s="6">
+        <f>F29/F37</f>
         <v>5.83072546230441</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="W29" s="6">
+        <f t="shared" si="5"/>
+        <v>16.873400673400674</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="str">
         <f>'Arduino Uno'!N7</f>
         <v>long</v>
@@ -3282,48 +4345,68 @@
         <f>'Arduino Due'!E11</f>
         <v>6.49</v>
       </c>
-      <c r="H30" s="6">
+      <c r="G30">
+        <f>'Teensy 3.1'!E11</f>
+        <v>1.99</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J30" s="6">
+        <f>C30/D30</f>
         <v>9.0346907993966816</v>
       </c>
-      <c r="I30" s="6">
+      <c r="K30" s="6">
+        <f>C30/E30</f>
+        <v>19.834437086092716</v>
+      </c>
+      <c r="L30" s="6">
+        <f>$C30/F30</f>
+        <v>18.459167950693374</v>
+      </c>
+      <c r="M30" s="6">
         <f t="shared" si="4"/>
-        <v>19.834437086092716</v>
-      </c>
-      <c r="J30" s="6">
-        <f t="shared" si="5"/>
-        <v>18.459167950693374</v>
-      </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6">
-        <f t="shared" si="6"/>
-        <v>2.1953642384105958</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="7"/>
-        <v>0.93066255778120177</v>
+        <v>60.201005025125625</v>
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="6">
+        <f>D30/E30</f>
+        <v>2.1953642384105958</v>
+      </c>
+      <c r="P30" s="6">
+        <f>E30/F30</f>
+        <v>0.93066255778120177</v>
+      </c>
+      <c r="Q30" s="6">
+        <f>E30/G30</f>
+        <v>3.0351758793969847</v>
+      </c>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6">
         <f>C30/C34</f>
         <v>2.9653465346534653</v>
       </c>
-      <c r="P30" s="6">
+      <c r="T30" s="6">
         <f>D30/D34</f>
         <v>1</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="U30" s="6">
         <f>E30/E34</f>
         <v>1</v>
       </c>
-      <c r="R30" s="6">
+      <c r="V30" s="6">
         <f>F30/F34</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="W30" s="6">
+        <f>G30/G34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="B31">
-        <f t="shared" ref="B31:B37" si="10">B27</f>
+        <f t="shared" ref="B31:B37" si="6">B27</f>
         <v>32</v>
       </c>
       <c r="C31" s="4">
@@ -3342,48 +4425,68 @@
         <f>'Arduino Due'!E12</f>
         <v>12.6</v>
       </c>
-      <c r="H31" s="6">
+      <c r="G31">
+        <f>'Teensy 3.1'!E12</f>
+        <v>3.82</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="6">
+        <f>C31/D31</f>
         <v>9.1187355435620656</v>
       </c>
-      <c r="I31" s="6">
+      <c r="K31" s="6">
+        <f>C31/E31</f>
+        <v>20.373815676141259</v>
+      </c>
+      <c r="L31" s="6">
+        <f>$C31/F31</f>
+        <v>18.773015873015872</v>
+      </c>
+      <c r="M31" s="6">
         <f t="shared" si="4"/>
-        <v>20.373815676141259</v>
-      </c>
-      <c r="J31" s="6">
-        <f t="shared" si="5"/>
-        <v>18.773015873015872</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6">
-        <f t="shared" si="6"/>
-        <v>2.2342807924203276</v>
-      </c>
-      <c r="M31" s="6">
-        <f t="shared" si="7"/>
-        <v>0.92142857142857137</v>
+        <v>61.921465968586389</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6">
-        <f t="shared" ref="O31:O33" si="11">C31/C35</f>
+        <f>D31/E31</f>
+        <v>2.2342807924203276</v>
+      </c>
+      <c r="P31" s="6">
+        <f>E31/F31</f>
+        <v>0.92142857142857137</v>
+      </c>
+      <c r="Q31" s="6">
+        <f>E31/G31</f>
+        <v>3.0392670157068062</v>
+      </c>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6">
+        <f>C31/C35</f>
         <v>3.0086491986771811</v>
       </c>
-      <c r="P31" s="6">
+      <c r="T31" s="6">
         <f>D31/D35</f>
         <v>1</v>
       </c>
-      <c r="Q31" s="6">
-        <f t="shared" ref="Q31:R33" si="12">E31/E35</f>
+      <c r="U31" s="6">
+        <f>E31/E35</f>
         <v>1</v>
       </c>
-      <c r="R31" s="6">
-        <f t="shared" si="12"/>
+      <c r="V31" s="6">
+        <f>F31/F35</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="W31" s="6">
+        <f t="shared" ref="W31:W33" si="7">G31/G35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="B32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="C32" s="4">
@@ -3402,48 +4505,68 @@
         <f>'Arduino Due'!E13</f>
         <v>24.8</v>
       </c>
-      <c r="H32" s="6">
+      <c r="G32">
+        <f>'Teensy 3.1'!E13</f>
+        <v>7.5</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="6">
+        <f>C32/D32</f>
         <v>8.7085417824717446</v>
       </c>
-      <c r="I32" s="6">
+      <c r="K32" s="6">
+        <f>C32/E32</f>
+        <v>20.650263620386642</v>
+      </c>
+      <c r="L32" s="6">
+        <f>$C32/F32</f>
+        <v>18.951612903225804</v>
+      </c>
+      <c r="M32" s="6">
         <f t="shared" si="4"/>
-        <v>20.650263620386642</v>
-      </c>
-      <c r="J32" s="6">
-        <f t="shared" si="5"/>
-        <v>18.951612903225804</v>
-      </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6">
-        <f t="shared" si="6"/>
-        <v>2.3712653778558872</v>
-      </c>
-      <c r="M32" s="6">
-        <f t="shared" si="7"/>
-        <v>0.91774193548387095</v>
+        <v>62.666666666666664</v>
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="6">
-        <f t="shared" si="11"/>
+        <f>D32/E32</f>
+        <v>2.3712653778558872</v>
+      </c>
+      <c r="P32" s="6">
+        <f>E32/F32</f>
+        <v>0.91774193548387095</v>
+      </c>
+      <c r="Q32" s="6">
+        <f>E32/G32</f>
+        <v>3.0346666666666668</v>
+      </c>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6">
+        <f>C32/C36</f>
         <v>3.0264005151320021</v>
       </c>
-      <c r="P32" s="6">
+      <c r="T32" s="6">
         <f>D32/D36</f>
         <v>1.0001853224610822</v>
       </c>
-      <c r="Q32" s="6">
-        <f t="shared" si="12"/>
+      <c r="U32" s="6">
+        <f>E32/E36</f>
         <v>1</v>
       </c>
-      <c r="R32" s="6">
-        <f t="shared" si="12"/>
+      <c r="V32" s="6">
+        <f>F32/F36</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="W32" s="6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
       <c r="B33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>128</v>
       </c>
       <c r="C33" s="4">
@@ -3462,52 +4585,72 @@
         <f>'Arduino Due'!E14</f>
         <v>49.21</v>
       </c>
-      <c r="H33" s="6">
+      <c r="G33">
+        <f>'Teensy 3.1'!E14</f>
+        <v>14.85</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J33" s="6">
+        <f>C33/D33</f>
         <v>8.7265952491849088</v>
       </c>
-      <c r="I33" s="6">
+      <c r="K33" s="6">
+        <f>C33/E33</f>
+        <v>20.790057700843317</v>
+      </c>
+      <c r="L33" s="6">
+        <f>$C33/F33</f>
+        <v>19.036781142044298</v>
+      </c>
+      <c r="M33" s="6">
         <f t="shared" si="4"/>
-        <v>20.790057700843317</v>
-      </c>
-      <c r="J33" s="6">
-        <f t="shared" si="5"/>
-        <v>19.036781142044298</v>
-      </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6">
-        <f t="shared" si="6"/>
-        <v>2.3823790501553481</v>
-      </c>
-      <c r="M33" s="6">
-        <f t="shared" si="7"/>
-        <v>0.91566754724649468</v>
+        <v>63.084175084175079</v>
       </c>
       <c r="N33" s="6"/>
       <c r="O33" s="6">
-        <f t="shared" si="11"/>
+        <f>D33/E33</f>
+        <v>2.3823790501553481</v>
+      </c>
+      <c r="P33" s="6">
+        <f>E33/F33</f>
+        <v>0.91566754724649468</v>
+      </c>
+      <c r="Q33" s="6">
+        <f>E33/G33</f>
+        <v>3.0343434343434348</v>
+      </c>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6">
+        <f>C33/C37</f>
         <v>3.0415584415584416</v>
       </c>
-      <c r="P33" s="6">
+      <c r="T33" s="6">
         <f>D33/D37</f>
         <v>1.000093161915409</v>
       </c>
-      <c r="Q33" s="6">
-        <f t="shared" si="12"/>
+      <c r="U33" s="6">
+        <f>E33/E37</f>
         <v>1</v>
       </c>
-      <c r="R33" s="6">
-        <f t="shared" si="12"/>
+      <c r="V33" s="6">
+        <f>F33/F37</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="W33" s="6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" t="str">
         <f>'Arduino Uno'!M7</f>
         <v>int</v>
       </c>
       <c r="B34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C34" s="4">
@@ -3526,36 +4669,52 @@
         <f>'Arduino Due'!F11</f>
         <v>6.49</v>
       </c>
-      <c r="H34" s="6">
+      <c r="G34">
+        <f>'Teensy 3.1'!F11</f>
+        <v>1.99</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="6">
+        <f>C34/D34</f>
         <v>3.0467571644042231</v>
       </c>
-      <c r="I34" s="6">
+      <c r="K34" s="6">
+        <f>C34/E34</f>
+        <v>6.6887417218543046</v>
+      </c>
+      <c r="L34" s="6">
+        <f>$C34/F34</f>
+        <v>6.2249614791987673</v>
+      </c>
+      <c r="M34" s="6">
         <f t="shared" si="4"/>
-        <v>6.6887417218543046</v>
-      </c>
-      <c r="J34" s="6">
-        <f t="shared" si="5"/>
-        <v>6.2249614791987673</v>
-      </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6">
+        <v>20.30150753768844</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6">
+        <f>D34/E34</f>
+        <v>2.1953642384105958</v>
+      </c>
+      <c r="P34" s="6">
+        <f>E34/F34</f>
+        <v>0.93066255778120177</v>
+      </c>
+      <c r="Q34" s="6">
+        <f>E34/G34</f>
+        <v>3.0351758793969847</v>
+      </c>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="B35">
         <f t="shared" si="6"/>
-        <v>2.1953642384105958</v>
-      </c>
-      <c r="M34" s="6">
-        <f t="shared" si="7"/>
-        <v>0.93066255778120177</v>
-      </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="B35">
-        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="C35" s="4">
@@ -3574,36 +4733,52 @@
         <f>'Arduino Due'!F12</f>
         <v>12.6</v>
       </c>
-      <c r="H35" s="6">
+      <c r="G35">
+        <f>'Teensy 3.1'!F12</f>
+        <v>3.82</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="6">
+        <f>C35/D35</f>
         <v>3.0308404009252121</v>
       </c>
-      <c r="I35" s="6">
+      <c r="K35" s="6">
+        <f>C35/E35</f>
+        <v>6.7717484926787259</v>
+      </c>
+      <c r="L35" s="6">
+        <f>$C35/F35</f>
+        <v>6.2396825396825406</v>
+      </c>
+      <c r="M35" s="6">
         <f t="shared" si="4"/>
-        <v>6.7717484926787259</v>
-      </c>
-      <c r="J35" s="6">
-        <f t="shared" si="5"/>
-        <v>6.2396825396825406</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6">
-        <f t="shared" si="6"/>
+        <v>20.581151832460733</v>
+      </c>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6">
+        <f>D35/E35</f>
         <v>2.2342807924203276</v>
       </c>
-      <c r="M35" s="6">
-        <f t="shared" si="7"/>
+      <c r="P35" s="6">
+        <f>E35/F35</f>
         <v>0.92142857142857137</v>
       </c>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
+      <c r="Q35" s="6">
+        <f>E35/G35</f>
+        <v>3.0392670157068062</v>
+      </c>
       <c r="R35" s="6"/>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+    </row>
+    <row r="36" spans="1:23">
       <c r="B36">
-        <f t="shared" si="10"/>
+        <f>B32</f>
         <v>64</v>
       </c>
       <c r="C36" s="4">
@@ -3622,36 +4797,52 @@
         <f>'Arduino Due'!F13</f>
         <v>24.8</v>
       </c>
-      <c r="H36" s="6">
+      <c r="G36">
+        <f>'Teensy 3.1'!F13</f>
+        <v>7.5</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="6">
+        <f>C36/D36</f>
         <v>2.8780578206078578</v>
       </c>
-      <c r="I36" s="6">
+      <c r="K36" s="6">
+        <f>C36/E36</f>
+        <v>6.8233743409490337</v>
+      </c>
+      <c r="L36" s="6">
+        <f>$C36/F36</f>
+        <v>6.2620967741935489</v>
+      </c>
+      <c r="M36" s="6">
         <f t="shared" si="4"/>
-        <v>6.8233743409490337</v>
-      </c>
-      <c r="J36" s="6">
-        <f t="shared" si="5"/>
-        <v>6.2620967741935489</v>
-      </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6">
+        <v>20.706666666666667</v>
+      </c>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6">
+        <f>D36/E36</f>
+        <v>2.3708260105448153</v>
+      </c>
+      <c r="P36" s="6">
+        <f>E36/F36</f>
+        <v>0.91774193548387095</v>
+      </c>
+      <c r="Q36" s="6">
+        <f>E36/G36</f>
+        <v>3.0346666666666668</v>
+      </c>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="B37">
         <f t="shared" si="6"/>
-        <v>2.3708260105448153</v>
-      </c>
-      <c r="M36" s="6">
-        <f t="shared" si="7"/>
-        <v>0.91774193548387095</v>
-      </c>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-    </row>
-    <row r="37" spans="1:18">
-      <c r="B37">
-        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="C37" s="4">
@@ -3670,49 +4861,375 @@
         <f>'Arduino Due'!F14</f>
         <v>49.21</v>
       </c>
-      <c r="H37" s="6">
+      <c r="G37">
+        <f>'Teensy 3.1'!F14</f>
+        <v>14.85</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="6">
+        <f>C37/D37</f>
         <v>2.8693869945966086</v>
       </c>
-      <c r="I37" s="6">
+      <c r="K37" s="6">
+        <f>C37/E37</f>
+        <v>6.8353306702174876</v>
+      </c>
+      <c r="L37" s="6">
+        <f>$C37/F37</f>
+        <v>6.2588904694167855</v>
+      </c>
+      <c r="M37" s="6">
         <f t="shared" si="4"/>
-        <v>6.8353306702174876</v>
-      </c>
-      <c r="J37" s="6">
-        <f t="shared" si="5"/>
-        <v>6.2588904694167855</v>
-      </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6">
-        <f t="shared" si="6"/>
+        <v>20.74074074074074</v>
+      </c>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6">
+        <f>D37/E37</f>
         <v>2.3821571238348866</v>
       </c>
-      <c r="M37" s="6">
-        <f t="shared" si="7"/>
+      <c r="P37" s="6">
+        <f>E37/F37</f>
         <v>0.91566754724649468</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
+      <c r="Q37" s="6">
+        <f>E37/G37</f>
+        <v>3.0343434343434348</v>
+      </c>
       <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" t="str">
+        <f>A26</f>
+        <v>float</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="8">
+        <f>1/(C27*0.000001)</f>
+        <v>1821.161901293025</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" ref="D39:G39" si="8">1/(D27*0.000001)</f>
+        <v>4454.5414049623596</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" si="8"/>
+        <v>12939.958592132507</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="8"/>
+        <v>13958.682300390843</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" si="8"/>
+        <v>16126.431220770844</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="9">
+        <f>$C$36/C28</f>
+        <v>0.13762850053172634</v>
+      </c>
+      <c r="J39" s="9">
+        <f t="shared" ref="J39:M39" si="9">$C$36/D28</f>
+        <v>0.34333340702584397</v>
+      </c>
+      <c r="K39" s="9">
+        <f t="shared" si="9"/>
+        <v>1.0024528789052416</v>
+      </c>
+      <c r="L39" s="9">
+        <f t="shared" si="9"/>
+        <v>1.0827581398591648</v>
+      </c>
+      <c r="M39" s="9">
+        <f t="shared" si="9"/>
+        <v>1.2434942749619666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="A40" t="str">
+        <f>A30</f>
+        <v>long</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="8">
+        <f>1/(C31*0.000001)</f>
+        <v>4227.6147797412705</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" ref="D40:G40" si="10">1/(D31*0.000001)</f>
+        <v>38550.501156515034</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="10"/>
+        <v>86132.644272179168</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="10"/>
+        <v>79365.079365079364</v>
+      </c>
+      <c r="G40" s="8">
+        <f t="shared" si="10"/>
+        <v>261780.10471204188</v>
+      </c>
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40" s="9">
+        <f>$C$36/C32</f>
+        <v>0.33042553191489366</v>
+      </c>
+      <c r="J40" s="9">
+        <f t="shared" ref="J40:M40" si="11">$C$36/D32</f>
+        <v>2.8775245506763021</v>
+      </c>
+      <c r="K40" s="9">
+        <f t="shared" si="11"/>
+        <v>6.8233743409490337</v>
+      </c>
+      <c r="L40" s="9">
+        <f t="shared" si="11"/>
+        <v>6.2620967741935489</v>
+      </c>
+      <c r="M40" s="9">
+        <f t="shared" si="11"/>
+        <v>20.706666666666667</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="A41" t="str">
+        <f>A34</f>
+        <v>int</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="8">
+        <f>1/(C35*0.000001)</f>
+        <v>12719.40981938438</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" ref="D41:G41" si="12">1/(D35*0.000001)</f>
+        <v>38550.501156515034</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="12"/>
+        <v>86132.644272179168</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="12"/>
+        <v>79365.079365079364</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="12"/>
+        <v>261780.10471204188</v>
+      </c>
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="9">
+        <f>$C$36/C36</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="9">
+        <f t="shared" ref="J41:M41" si="13">$C$36/D36</f>
+        <v>2.8780578206078578</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="13"/>
+        <v>6.8233743409490337</v>
+      </c>
+      <c r="L41" s="9">
+        <f t="shared" si="13"/>
+        <v>6.2620967741935489</v>
+      </c>
+      <c r="M41" s="9">
+        <f t="shared" si="13"/>
+        <v>20.706666666666667</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59">
+        <v>250</v>
+      </c>
+      <c r="H59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="C60" t="str">
+        <f>C23</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" ref="D60:G60" si="14">D23</f>
+        <v>Arduino M0 Pro</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="14"/>
+        <v>Maple</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="14"/>
+        <v>Arduino Due</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="14"/>
+        <v>Teensy 3.1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" t="str">
+        <f>A26</f>
+        <v>float</v>
+      </c>
+      <c r="C61" s="8">
+        <f>SQRT($G$59/((C28*0.000001)/$B28))</f>
+        <v>3765.5502941905706</v>
+      </c>
+      <c r="D61" s="8">
+        <f t="shared" ref="D61:G61" si="15">SQRT($G$59/((D28*0.000001)/$B28))</f>
+        <v>5947.4704793272776</v>
+      </c>
+      <c r="E61" s="8">
+        <f t="shared" si="15"/>
+        <v>10162.633113501566</v>
+      </c>
+      <c r="F61" s="8">
+        <f t="shared" si="15"/>
+        <v>10561.849922156138</v>
+      </c>
+      <c r="G61" s="8">
+        <f t="shared" si="15"/>
+        <v>11318.689818636485</v>
+      </c>
+      <c r="H61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" t="str">
+        <f>A30</f>
+        <v>long</v>
+      </c>
+      <c r="C62" s="8">
+        <f>SQRT($G$59/((C32*0.000001)/$B32))</f>
+        <v>5834.5996599157825</v>
+      </c>
+      <c r="D62" s="8">
+        <f t="shared" ref="D62:G62" si="16">SQRT($G$59/((D32*0.000001)/$B32))</f>
+        <v>17218.042770596836</v>
+      </c>
+      <c r="E62" s="8">
+        <f t="shared" si="16"/>
+        <v>26513.915171382934</v>
+      </c>
+      <c r="F62" s="8">
+        <f t="shared" si="16"/>
+        <v>25400.025400038103</v>
+      </c>
+      <c r="G62" s="8">
+        <f t="shared" si="16"/>
+        <v>46188.021535170061</v>
+      </c>
+      <c r="H62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" t="str">
+        <f>A34</f>
+        <v>int</v>
+      </c>
+      <c r="C63" s="8">
+        <f>SQRT($G$59/((C36*0.000001)/$B36))</f>
+        <v>10150.192141783918</v>
+      </c>
+      <c r="D63" s="8">
+        <f t="shared" ref="D63:G63" si="17">SQRT($G$59/((D36*0.000001)/$B36))</f>
+        <v>17219.638141716368</v>
+      </c>
+      <c r="E63" s="8">
+        <f t="shared" si="17"/>
+        <v>26513.915171382934</v>
+      </c>
+      <c r="F63" s="8">
+        <f t="shared" si="17"/>
+        <v>25400.025400038103</v>
+      </c>
+      <c r="G63" s="8">
+        <f t="shared" si="17"/>
+        <v>46188.021535170061</v>
+      </c>
+      <c r="H63" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C26:F37">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="C26:G37">
+    <cfRule type="cellIs" dxfId="4" priority="11" stopIfTrue="1" operator="lessThan">
+      <formula>$D$21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="12" stopIfTrue="1" operator="lessThan">
+      <formula>$D$20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" stopIfTrue="1" operator="lessThan">
+      <formula>$D$19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>$D$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>$D$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="lessThan">
-      <formula>$D$19</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:G41">
+    <cfRule type="cellIs" dxfId="14" priority="6" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="lessThan">
-      <formula>$D$20</formula>
+    <cfRule type="cellIs" dxfId="13" priority="7" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="lessThan">
-      <formula>$D$21</formula>
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="lessThan">
+      <formula>$C$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:G63">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$19</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThan">
+      <formula>$C$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="lessThan">
+      <formula>$C$18</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4827,7 +6344,7 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5011,4 +6528,682 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>11.78</v>
+      </c>
+      <c r="D9">
+        <v>6.81</v>
+      </c>
+      <c r="E9">
+        <v>0.61</v>
+      </c>
+      <c r="F9">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>24.81</v>
+      </c>
+      <c r="D10">
+        <v>14.74</v>
+      </c>
+      <c r="E10">
+        <v>1.07</v>
+      </c>
+      <c r="F10">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>50.7</v>
+      </c>
+      <c r="D11">
+        <v>30.53</v>
+      </c>
+      <c r="E11">
+        <v>1.99</v>
+      </c>
+      <c r="F11">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>102.3</v>
+      </c>
+      <c r="D12">
+        <v>62.01</v>
+      </c>
+      <c r="E12">
+        <v>3.82</v>
+      </c>
+      <c r="F12">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>205.35</v>
+      </c>
+      <c r="D13">
+        <v>124.89</v>
+      </c>
+      <c r="E13">
+        <v>7.5</v>
+      </c>
+      <c r="F13">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>411.28</v>
+      </c>
+      <c r="D14">
+        <v>250.57</v>
+      </c>
+      <c r="E14">
+        <v>14.85</v>
+      </c>
+      <c r="F14">
+        <v>14.85</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>822.97</v>
+      </c>
+      <c r="D15">
+        <v>501.85</v>
+      </c>
+      <c r="E15">
+        <v>29.55</v>
+      </c>
+      <c r="F15">
+        <v>29.55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16">
+        <v>512</v>
+      </c>
+      <c r="C16">
+        <v>1646.22</v>
+      </c>
+      <c r="D16">
+        <v>1004.33</v>
+      </c>
+      <c r="E16">
+        <v>58.96</v>
+      </c>
+      <c r="F16">
+        <v>58.96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19">
+        <f>96/72</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>12.67</v>
+      </c>
+      <c r="D21">
+        <v>7.36</v>
+      </c>
+      <c r="E21">
+        <v>0.81</v>
+      </c>
+      <c r="F21">
+        <v>0.81</v>
+      </c>
+      <c r="H21">
+        <f>F21/F9</f>
+        <v>1.3278688524590165</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>26.53</v>
+      </c>
+      <c r="D22">
+        <v>15.51</v>
+      </c>
+      <c r="E22">
+        <v>1.42</v>
+      </c>
+      <c r="F22">
+        <v>1.42</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:H28" si="0">F22/F10</f>
+        <v>1.3271028037383177</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>54.1</v>
+      </c>
+      <c r="D23">
+        <v>31.67</v>
+      </c>
+      <c r="E23">
+        <v>2.65</v>
+      </c>
+      <c r="F23">
+        <v>2.65</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1.3316582914572863</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>109.06</v>
+      </c>
+      <c r="D24">
+        <v>63.87</v>
+      </c>
+      <c r="E24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>1.3350785340314135</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25">
+        <v>64</v>
+      </c>
+      <c r="C25">
+        <v>218.82</v>
+      </c>
+      <c r="D25">
+        <v>128.22</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26">
+        <v>128</v>
+      </c>
+      <c r="C26">
+        <v>438.17</v>
+      </c>
+      <c r="D26">
+        <v>256.58</v>
+      </c>
+      <c r="E26">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="F26">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>1.3340067340067339</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27">
+        <v>256</v>
+      </c>
+      <c r="C27">
+        <v>876.73</v>
+      </c>
+      <c r="D27">
+        <v>513.32000000000005</v>
+      </c>
+      <c r="E27">
+        <v>39.43</v>
+      </c>
+      <c r="F27">
+        <v>39.43</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1.3343485617597293</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28">
+        <v>512</v>
+      </c>
+      <c r="C28">
+        <v>1753.6</v>
+      </c>
+      <c r="D28">
+        <v>1026.67</v>
+      </c>
+      <c r="E28">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="F28">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>1.3339552238805972</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>12.36</v>
+      </c>
+      <c r="D33">
+        <v>7.95</v>
+      </c>
+      <c r="E33">
+        <v>0.89</v>
+      </c>
+      <c r="F33">
+        <v>0.89</v>
+      </c>
+      <c r="H33">
+        <f>C33/C9</f>
+        <v>1.0492359932088284</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:K40" si="1">D33/D9</f>
+        <v>1.1674008810572689</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>1.459016393442623</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>1.459016393442623</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>25.72</v>
+      </c>
+      <c r="D34">
+        <v>16.88</v>
+      </c>
+      <c r="E34">
+        <v>1.56</v>
+      </c>
+      <c r="F34">
+        <v>1.56</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:H40" si="2">C34/C10</f>
+        <v>1.0366787585650947</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>1.1451831750339212</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>1.4579439252336448</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>1.4579439252336448</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>52.28</v>
+      </c>
+      <c r="D35">
+        <v>34.659999999999997</v>
+      </c>
+      <c r="E35">
+        <v>2.89</v>
+      </c>
+      <c r="F35">
+        <v>2.89</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>1.031163708086785</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>1.1352767769407139</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>1.4522613065326633</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>1.4522613065326633</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>105.2</v>
+      </c>
+      <c r="D36">
+        <v>70.22</v>
+      </c>
+      <c r="E36">
+        <v>5.56</v>
+      </c>
+      <c r="F36">
+        <v>5.56</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>1.0283479960899315</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>1.1323980003225287</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>1.4554973821989527</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>1.4554973821989527</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>210.9</v>
+      </c>
+      <c r="D37">
+        <v>141.04</v>
+      </c>
+      <c r="E37">
+        <v>10.91</v>
+      </c>
+      <c r="F37">
+        <v>10.91</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>1.027027027027027</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>1.1293137961406037</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>1.4546666666666668</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>1.4546666666666668</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>422.11</v>
+      </c>
+      <c r="D38">
+        <v>282.75</v>
+      </c>
+      <c r="E38">
+        <v>21.6</v>
+      </c>
+      <c r="F38">
+        <v>21.6</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>1.0263324255981328</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>1.1284271860158839</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>1.4545454545454546</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>1.4545454545454546</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39">
+        <v>256</v>
+      </c>
+      <c r="C39">
+        <v>844.39</v>
+      </c>
+      <c r="D39">
+        <v>566.07000000000005</v>
+      </c>
+      <c r="E39">
+        <v>42.97</v>
+      </c>
+      <c r="F39">
+        <v>42.97</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>1.026027680231357</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>1.1279665238617118</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>1.4541455160744501</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>1.4541455160744501</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40">
+        <v>512</v>
+      </c>
+      <c r="C40">
+        <v>1688.76</v>
+      </c>
+      <c r="D40">
+        <v>1132.6500000000001</v>
+      </c>
+      <c r="E40">
+        <v>85.71</v>
+      </c>
+      <c r="F40">
+        <v>85.71</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>1.0258410176039654</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>1.127766769886392</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>1.4536974219810039</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>1.4536974219810039</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>